<commit_message>
add 2 class variables to track instances
</commit_message>
<xml_diff>
--- a/classes+unitTests/stockAnalysis/Book1.xlsx
+++ b/classes+unitTests/stockAnalysis/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zimul\Documents\python\classes+unitTests\stockAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F12BDE-F9C3-4C90-97A6-19AA0E95D5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366EAE8C-8B50-4586-87B3-6F03D1DD792D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{59D6CB83-70A6-4510-8AD0-4832DF31627A}"/>
+    <workbookView xWindow="4725" yWindow="225" windowWidth="21600" windowHeight="11835" xr2:uid="{59D6CB83-70A6-4510-8AD0-4832DF31627A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
   <si>
     <t>Symbol</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>goo</t>
+  </si>
+  <si>
+    <t>se</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87510DCF-C091-4DC8-B73D-768B648EB4C7}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +513,50 @@
         <v>80</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41244</v>
+      </c>
+      <c r="C10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41245</v>
+      </c>
+      <c r="C11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41246</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41247</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>